<commit_message>
Updated version of data processing scripts
Better treatment of uncertainties, removed conversion to M0 reference
</commit_message>
<xml_diff>
--- a/references_nitrate.xlsx
+++ b/references_nitrate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacksaville/Documents/Lab/Orbitrap/2401 tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacksaville/Desktop/data 240913/240904_stds+blanks_norein_NO3_conc_noM0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F1AFEC-6A89-9F4C-BC23-FEA91E56D964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62436B54-503D-2142-943A-B7A7D3F7E100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="760" windowWidth="27640" windowHeight="15880" xr2:uid="{90F8ED79-F1DF-4C49-B0DD-9D7371D6F505}"/>
+    <workbookView xWindow="1180" yWindow="1600" windowWidth="44060" windowHeight="19560" xr2:uid="{90F8ED79-F1DF-4C49-B0DD-9D7371D6F505}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>USGS34</t>
   </si>
@@ -86,22 +86,34 @@
     <t>sample_name</t>
   </si>
   <si>
-    <t>mean_d15N18O</t>
-  </si>
-  <si>
-    <t>mean_d17O18O</t>
-  </si>
-  <si>
-    <t>mean_d18O18O</t>
-  </si>
-  <si>
-    <t>err_d17O18O</t>
-  </si>
-  <si>
     <t>err_d18O18O</t>
   </si>
   <si>
-    <t>err_d15N18O</t>
+    <t>mean_d18O/15N</t>
+  </si>
+  <si>
+    <t>mean_d17O/15N</t>
+  </si>
+  <si>
+    <t>mean_d15N18O/15N</t>
+  </si>
+  <si>
+    <t>mean_d17O18O/15N</t>
+  </si>
+  <si>
+    <t>err_d18O/15N</t>
+  </si>
+  <si>
+    <t>err_d17O/15N</t>
+  </si>
+  <si>
+    <t>err_d15N18O/15N</t>
+  </si>
+  <si>
+    <t>err_d17O18O/15N</t>
+  </si>
+  <si>
+    <t>mean_d18O18O/15N</t>
   </si>
 </sst>
 </file>
@@ -111,10 +123,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,10 +159,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,21 +480,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858B4891-00C2-C246-95BF-C212447929C6}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="M1" sqref="M1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -486,104 +513,151 @@
         <v>11</v>
       </c>
       <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>-1.8</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>-14.8</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>-27.9</v>
       </c>
-      <c r="H2" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0.3</v>
-      </c>
+      <c r="E2" s="3">
+        <f>1000*((D2+1000)/(B2+1000)-1)</f>
+        <v>-26.147064716489755</v>
+      </c>
+      <c r="F2" s="3">
+        <f>1000*((C2+1000)/(B2+1000)-1)</f>
+        <v>-13.02344219595275</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="4"/>
       <c r="J2" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="M2" s="2">
+        <f>SQRT(J2^2+L2^2)</f>
+        <v>0.42426406871192851</v>
+      </c>
+      <c r="N2" s="2">
+        <f>SQRT(K2^2+L2^2)</f>
+        <v>0.42426406871192851</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>2.7</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>51.5</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <v>57.5</v>
       </c>
-      <c r="E3" s="2">
-        <f>1000*((1+B3/1000)*(1+D3/1000)-1)</f>
-        <v>60.35524999999997</v>
-      </c>
-      <c r="F3" s="2">
-        <f>1000*((1+C3/1000)*(1+(2/3)*D3/1000)-1)</f>
-        <v>91.807500000000047</v>
-      </c>
-      <c r="G3" s="2">
-        <f>1000*((1+D3/1000)*(1+(2/3)*D3/1000)-1)</f>
-        <v>98.037499999999994</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.3</v>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E10" si="0">1000*((D3+1000)/(B3+1000)-1)</f>
+        <v>54.652438416276098</v>
+      </c>
+      <c r="F3" s="3">
+        <f>1000*((C3+1000)/(B3+1000)-1)</f>
+        <v>48.668594794055942</v>
+      </c>
+      <c r="G3" s="3">
+        <f>D3</f>
+        <v>57.5</v>
+      </c>
+      <c r="H3" s="3">
+        <f>((1000+C3)*(1000+E3)/1000)-1000</f>
+        <v>108.96703899471413</v>
+      </c>
+      <c r="I3" s="3">
+        <f>((1000+D3)*(1000+E3)/1000)-1000</f>
+        <v>115.29495362521197</v>
       </c>
       <c r="J3" s="1">
         <v>0.3</v>
       </c>
-      <c r="K3" s="2">
-        <f>SQRT(H3^2+J3^2)</f>
-        <v>0.42426406871192851</v>
-      </c>
-      <c r="L3" s="2">
-        <f>SQRT(I3^2+((2/3)*J3)^2)</f>
-        <v>0.36055512754639896</v>
+      <c r="K3" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.3</v>
       </c>
       <c r="M3" s="2">
-        <f>SQRT(J3^2+((2/3)*J3)^2)</f>
-        <v>0.36055512754639896</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+        <f>SQRT(J3^2+L3^2)</f>
+        <v>0.42426406871192851</v>
+      </c>
+      <c r="N3" s="2">
+        <f>SQRT(K3^2+L3^2)</f>
+        <v>0.42426406871192851</v>
+      </c>
+      <c r="O3" s="2">
+        <f>SQRT(L3^2+(J3)^2)</f>
+        <v>0.42426406871192851</v>
+      </c>
+      <c r="P3" s="2">
+        <f>SQRT(J2^2+L2^2)</f>
+        <v>0.42426406871192851</v>
+      </c>
+      <c r="Q3" s="2">
+        <f>SQRT(J2^2+L2^2)</f>
+        <v>0.42426406871192851</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -594,15 +668,23 @@
       <c r="D4" s="1">
         <v>25.7</v>
       </c>
-      <c r="H4" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="I4" s="1"/>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>-130.7627118644067</v>
+      </c>
       <c r="J4" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" ref="M4:M10" si="1">SQRT(J4^2+L4^2)</f>
+        <v>0.42426406871192851</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -613,15 +695,23 @@
       <c r="D5" s="1">
         <v>22.9</v>
       </c>
-      <c r="H5" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="I5" s="1"/>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>32.919317378572231</v>
+      </c>
       <c r="J5" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K5" s="1"/>
+      <c r="L5" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" si="1"/>
+        <v>0.42426406871192851</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -632,15 +722,23 @@
       <c r="D6" s="1">
         <v>33</v>
       </c>
-      <c r="H6" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="I6" s="1"/>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.63850782655816563</v>
+      </c>
       <c r="J6" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K6" s="1"/>
+      <c r="L6" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="1"/>
+        <v>0.42426406871192851</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -651,15 +749,23 @@
       <c r="D7" s="1">
         <v>-6.9</v>
       </c>
-      <c r="H7" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="I7" s="1"/>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>-4.1214989821601877</v>
+      </c>
       <c r="J7" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K7" s="1"/>
+      <c r="L7" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.42426406871192851</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -670,15 +776,23 @@
       <c r="D8" s="1">
         <v>52.4</v>
       </c>
-      <c r="H8" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="I8" s="1"/>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>54.297735924664359</v>
+      </c>
       <c r="J8" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K8" s="1"/>
+      <c r="L8" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.42426406871192851</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -689,15 +803,23 @@
       <c r="D9" s="1">
         <v>3.13</v>
       </c>
-      <c r="H9" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="I9" s="1"/>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>1.9977425509174473</v>
+      </c>
       <c r="J9" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K9" s="1"/>
+      <c r="L9" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.42426406871192851</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -708,12 +830,20 @@
       <c r="D10" s="1">
         <v>32.869999999999997</v>
       </c>
-      <c r="H10" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="I10" s="1"/>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.80294089194177243</v>
+      </c>
       <c r="J10" s="1">
         <v>0.3</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.42426406871192851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>